<commit_message>
Added code for precipitation comparison graphs
</commit_message>
<xml_diff>
--- a/data/amnhsize.xlsx
+++ b/data/amnhsize.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aswop\OneDrive\Documents\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMASH Scholar\Documents\Lasioglossum-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECC2BD5-0025-41EC-8715-D1F9390AEA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6F9BC0-3F61-4B7D-8014-C74C4943C9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B5684E87-1B8A-4B85-A4A9-074F08A5F36F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="232">
   <si>
     <t>id</t>
   </si>
@@ -726,6 +726,12 @@
   </si>
   <si>
     <t>matybc</t>
+  </si>
+  <si>
+    <t>precip</t>
+  </si>
+  <si>
+    <t>precipybc</t>
   </si>
 </sst>
 </file>
@@ -1101,15 +1107,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A84B6BF-08AE-4479-BFF7-34F35A33A8E2}">
-  <dimension ref="A1:AJ58"/>
+  <dimension ref="A1:AL550"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1212,8 +1218,14 @@
       <c r="AJ1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1722944</v>
       </c>
@@ -1314,8 +1326,14 @@
       <c r="AJ2">
         <v>15.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK2">
+        <v>292</v>
+      </c>
+      <c r="AL2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1759970</v>
       </c>
@@ -1416,8 +1434,14 @@
       <c r="AJ3">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK3">
+        <v>339</v>
+      </c>
+      <c r="AL3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1806723</v>
       </c>
@@ -1518,8 +1542,14 @@
       <c r="AJ4">
         <v>22.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK4">
+        <v>299</v>
+      </c>
+      <c r="AL4">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1807982</v>
       </c>
@@ -1620,8 +1650,14 @@
       <c r="AJ5">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK5">
+        <v>337</v>
+      </c>
+      <c r="AL5">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1807988</v>
       </c>
@@ -1722,8 +1758,14 @@
       <c r="AJ6">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK6">
+        <v>313</v>
+      </c>
+      <c r="AL6">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1807990</v>
       </c>
@@ -1824,8 +1866,14 @@
       <c r="AJ7">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK7">
+        <v>339</v>
+      </c>
+      <c r="AL7">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1906828</v>
       </c>
@@ -1926,8 +1974,14 @@
       <c r="AJ8">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK8">
+        <v>287</v>
+      </c>
+      <c r="AL8">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1906831</v>
       </c>
@@ -2028,8 +2082,14 @@
       <c r="AJ9">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK9">
+        <v>328</v>
+      </c>
+      <c r="AL9">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1906836</v>
       </c>
@@ -2130,8 +2190,14 @@
       <c r="AJ10">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK10">
+        <v>328</v>
+      </c>
+      <c r="AL10">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1906841</v>
       </c>
@@ -2232,8 +2298,14 @@
       <c r="AJ11">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK11">
+        <v>328</v>
+      </c>
+      <c r="AL11">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1906842</v>
       </c>
@@ -2334,8 +2406,14 @@
       <c r="AJ12">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK12">
+        <v>328</v>
+      </c>
+      <c r="AL12">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1906843</v>
       </c>
@@ -2436,8 +2514,14 @@
       <c r="AJ13">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK13">
+        <v>328</v>
+      </c>
+      <c r="AL13">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1906855</v>
       </c>
@@ -2538,8 +2622,14 @@
       <c r="AJ14">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK14">
+        <v>328</v>
+      </c>
+      <c r="AL14">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1906886</v>
       </c>
@@ -2640,8 +2730,14 @@
       <c r="AJ15">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK15">
+        <v>328</v>
+      </c>
+      <c r="AL15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1906890</v>
       </c>
@@ -2742,8 +2838,14 @@
       <c r="AJ16">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK16">
+        <v>328</v>
+      </c>
+      <c r="AL16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1906899</v>
       </c>
@@ -2844,8 +2946,14 @@
       <c r="AJ17">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK17">
+        <v>328</v>
+      </c>
+      <c r="AL17">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1906908</v>
       </c>
@@ -2946,8 +3054,14 @@
       <c r="AJ18">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK18">
+        <v>476</v>
+      </c>
+      <c r="AL18">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1906913</v>
       </c>
@@ -3048,8 +3162,14 @@
       <c r="AJ19">
         <v>18.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK19">
+        <v>311</v>
+      </c>
+      <c r="AL19">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1907695</v>
       </c>
@@ -3150,8 +3270,14 @@
       <c r="AJ20">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK20">
+        <v>311</v>
+      </c>
+      <c r="AL20">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1907704</v>
       </c>
@@ -3252,8 +3378,14 @@
       <c r="AJ21">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK21">
+        <v>225</v>
+      </c>
+      <c r="AL21">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1907746</v>
       </c>
@@ -3354,8 +3486,14 @@
       <c r="AJ22">
         <v>21.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK22">
+        <v>225</v>
+      </c>
+      <c r="AL22">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1907753</v>
       </c>
@@ -3456,8 +3594,14 @@
       <c r="AJ23">
         <v>13.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK23">
+        <v>225</v>
+      </c>
+      <c r="AL23">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1907771</v>
       </c>
@@ -3558,8 +3702,14 @@
       <c r="AJ24">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK24">
+        <v>225</v>
+      </c>
+      <c r="AL24">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1907776</v>
       </c>
@@ -3660,8 +3810,14 @@
       <c r="AJ25">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK25">
+        <v>238</v>
+      </c>
+      <c r="AL25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1907798</v>
       </c>
@@ -3762,8 +3918,14 @@
       <c r="AJ26">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK26">
+        <v>347</v>
+      </c>
+      <c r="AL26">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1907807</v>
       </c>
@@ -3864,8 +4026,14 @@
       <c r="AJ27">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK27">
+        <v>325</v>
+      </c>
+      <c r="AL27">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1907808</v>
       </c>
@@ -3966,8 +4134,14 @@
       <c r="AJ28">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK28">
+        <v>325</v>
+      </c>
+      <c r="AL28">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1907812</v>
       </c>
@@ -4068,8 +4242,14 @@
       <c r="AJ29">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK29">
+        <v>284</v>
+      </c>
+      <c r="AL29">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1907815</v>
       </c>
@@ -4170,8 +4350,14 @@
       <c r="AJ30">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK30">
+        <v>339</v>
+      </c>
+      <c r="AL30">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1907817</v>
       </c>
@@ -4272,8 +4458,14 @@
       <c r="AJ31">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK31">
+        <v>339</v>
+      </c>
+      <c r="AL31">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1907818</v>
       </c>
@@ -4374,8 +4566,14 @@
       <c r="AJ32">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK32">
+        <v>339</v>
+      </c>
+      <c r="AL32">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1907822</v>
       </c>
@@ -4476,8 +4674,14 @@
       <c r="AJ33">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK33">
+        <v>339</v>
+      </c>
+      <c r="AL33">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1907825</v>
       </c>
@@ -4578,8 +4782,14 @@
       <c r="AJ34">
         <v>10.7</v>
       </c>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK34">
+        <v>339</v>
+      </c>
+      <c r="AL34">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1907827</v>
       </c>
@@ -4680,8 +4890,14 @@
       <c r="AJ35">
         <v>10.7</v>
       </c>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK35">
+        <v>339</v>
+      </c>
+      <c r="AL35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1907831</v>
       </c>
@@ -4782,8 +4998,14 @@
       <c r="AJ36">
         <v>18.2</v>
       </c>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK36">
+        <v>339</v>
+      </c>
+      <c r="AL36">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1907834</v>
       </c>
@@ -4884,8 +5106,14 @@
       <c r="AJ37">
         <v>18.2</v>
       </c>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK37">
+        <v>339</v>
+      </c>
+      <c r="AL37">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1907853</v>
       </c>
@@ -4986,8 +5214,14 @@
       <c r="AJ38">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK38">
+        <v>339</v>
+      </c>
+      <c r="AL38">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1907865</v>
       </c>
@@ -5088,8 +5322,14 @@
       <c r="AJ39">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK39">
+        <v>339</v>
+      </c>
+      <c r="AL39">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>1907875</v>
       </c>
@@ -5193,8 +5433,14 @@
       <c r="AJ40" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK40">
+        <v>339</v>
+      </c>
+      <c r="AL40">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>1907925</v>
       </c>
@@ -5298,8 +5544,14 @@
       <c r="AJ41" s="3">
         <v>12.3</v>
       </c>
-    </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK41">
+        <v>339</v>
+      </c>
+      <c r="AL41">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>1907940</v>
       </c>
@@ -5403,8 +5655,14 @@
       <c r="AJ42" s="3">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK42">
+        <v>339</v>
+      </c>
+      <c r="AL42">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>1907941</v>
       </c>
@@ -5508,8 +5766,14 @@
       <c r="AJ43" s="3">
         <v>10.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK43">
+        <v>418</v>
+      </c>
+      <c r="AL43">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>1907946</v>
       </c>
@@ -5613,8 +5877,14 @@
       <c r="AJ44" s="3">
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK44">
+        <v>279</v>
+      </c>
+      <c r="AL44">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>1907948</v>
       </c>
@@ -5718,8 +5988,14 @@
       <c r="AJ45" s="3">
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK45">
+        <v>298</v>
+      </c>
+      <c r="AL45">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>1907952</v>
       </c>
@@ -5823,8 +6099,14 @@
       <c r="AJ46" s="3">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK46">
+        <v>339</v>
+      </c>
+      <c r="AL46">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>1907953</v>
       </c>
@@ -5928,8 +6210,14 @@
       <c r="AJ47" s="3">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK47">
+        <v>339</v>
+      </c>
+      <c r="AL47">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>1907959</v>
       </c>
@@ -6033,8 +6321,14 @@
       <c r="AJ48" s="3">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK48">
+        <v>339</v>
+      </c>
+      <c r="AL48">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>1907962</v>
       </c>
@@ -6138,8 +6432,14 @@
       <c r="AJ49" s="3">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK49">
+        <v>339</v>
+      </c>
+      <c r="AL49">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>1907964</v>
       </c>
@@ -6243,8 +6543,14 @@
       <c r="AJ50" s="3">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK50">
+        <v>339</v>
+      </c>
+      <c r="AL50">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>1907967</v>
       </c>
@@ -6348,8 +6654,14 @@
       <c r="AJ51" s="3">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK51">
+        <v>339</v>
+      </c>
+      <c r="AL51">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>1907969</v>
       </c>
@@ -6453,8 +6765,14 @@
       <c r="AJ52" s="3">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK52">
+        <v>339</v>
+      </c>
+      <c r="AL52">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>1907971</v>
       </c>
@@ -6558,8 +6876,14 @@
       <c r="AJ53" s="3">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK53">
+        <v>339</v>
+      </c>
+      <c r="AL53">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>1907975</v>
       </c>
@@ -6663,8 +6987,14 @@
       <c r="AJ54" s="3">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK54">
+        <v>298</v>
+      </c>
+      <c r="AL54">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>1907978</v>
       </c>
@@ -6768,8 +7098,14 @@
       <c r="AJ55" s="3">
         <v>10.9</v>
       </c>
-    </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK55">
+        <v>508</v>
+      </c>
+      <c r="AL55">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>1907979</v>
       </c>
@@ -6873,8 +7209,14 @@
       <c r="AJ56" s="3">
         <v>10.9</v>
       </c>
-    </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK56">
+        <v>366</v>
+      </c>
+      <c r="AL56">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>1907980</v>
       </c>
@@ -6978,8 +7320,14 @@
       <c r="AJ57" s="3">
         <v>10.9</v>
       </c>
-    </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK57">
+        <v>339</v>
+      </c>
+      <c r="AL57">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>1907981</v>
       </c>
@@ -7082,6 +7430,3948 @@
       </c>
       <c r="AJ58" s="3">
         <v>11</v>
+      </c>
+      <c r="AK58">
+        <v>339</v>
+      </c>
+      <c r="AL58">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK59">
+        <v>339</v>
+      </c>
+      <c r="AL59">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK60">
+        <v>339</v>
+      </c>
+      <c r="AL60">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK61">
+        <v>339</v>
+      </c>
+      <c r="AL61">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK62">
+        <v>339</v>
+      </c>
+      <c r="AL62">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK63">
+        <v>508</v>
+      </c>
+      <c r="AL63">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK64">
+        <v>508</v>
+      </c>
+      <c r="AL64">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="65" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK65">
+        <v>508</v>
+      </c>
+      <c r="AL65">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="66" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK66">
+        <v>363</v>
+      </c>
+      <c r="AL66">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="67" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK67">
+        <v>396</v>
+      </c>
+      <c r="AL67">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="68" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK68">
+        <v>646</v>
+      </c>
+      <c r="AL68">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="69" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK69">
+        <v>325</v>
+      </c>
+      <c r="AL69">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="70" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK70">
+        <v>463</v>
+      </c>
+      <c r="AL70">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="71" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK71">
+        <v>385</v>
+      </c>
+      <c r="AL71">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="72" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK72">
+        <v>401</v>
+      </c>
+      <c r="AL72">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="73" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK73">
+        <v>401</v>
+      </c>
+      <c r="AL73">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="74" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK74">
+        <v>102</v>
+      </c>
+      <c r="AL74">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK75">
+        <v>140</v>
+      </c>
+      <c r="AL75">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="76" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK76">
+        <v>320</v>
+      </c>
+      <c r="AL76">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="77" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK77">
+        <v>320</v>
+      </c>
+      <c r="AL77">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="78" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK78">
+        <v>409</v>
+      </c>
+      <c r="AL78">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="79" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK79">
+        <v>294</v>
+      </c>
+      <c r="AL79">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="80" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK80">
+        <v>294</v>
+      </c>
+      <c r="AL80">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="81" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK81">
+        <v>294</v>
+      </c>
+      <c r="AL81">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK82">
+        <v>294</v>
+      </c>
+      <c r="AL82">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="83" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK83">
+        <v>314</v>
+      </c>
+      <c r="AL83">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="84" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK84">
+        <v>382</v>
+      </c>
+      <c r="AL84">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="85" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK85">
+        <v>422</v>
+      </c>
+      <c r="AL85">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="86" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK86">
+        <v>424</v>
+      </c>
+      <c r="AL86">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="87" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK87">
+        <v>457</v>
+      </c>
+      <c r="AL87">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="88" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK88">
+        <v>324</v>
+      </c>
+      <c r="AL88">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="89" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK89">
+        <v>476</v>
+      </c>
+      <c r="AL89">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="90" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK90">
+        <v>128</v>
+      </c>
+      <c r="AL90">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="91" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK91">
+        <v>280</v>
+      </c>
+      <c r="AL91">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="92" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK92">
+        <v>112</v>
+      </c>
+      <c r="AL92">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK93">
+        <v>379</v>
+      </c>
+      <c r="AL93">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="94" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK94">
+        <v>379</v>
+      </c>
+      <c r="AL94">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="95" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK95">
+        <v>379</v>
+      </c>
+      <c r="AL95">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="96" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK96">
+        <v>205</v>
+      </c>
+      <c r="AL96">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="97" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK97">
+        <v>205</v>
+      </c>
+      <c r="AL97">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="98" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK98">
+        <v>205</v>
+      </c>
+      <c r="AL98">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="99" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK99">
+        <v>205</v>
+      </c>
+      <c r="AL99">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="100" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK100">
+        <v>274</v>
+      </c>
+      <c r="AL100">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="101" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK101">
+        <v>274</v>
+      </c>
+      <c r="AL101">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="102" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK102">
+        <v>340</v>
+      </c>
+      <c r="AL102">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="103" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK103">
+        <v>310</v>
+      </c>
+      <c r="AL103">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="104" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK104">
+        <v>310</v>
+      </c>
+      <c r="AL104">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="105" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK105">
+        <v>310</v>
+      </c>
+      <c r="AL105">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="106" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK106">
+        <v>301</v>
+      </c>
+      <c r="AL106">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="107" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK107">
+        <v>661</v>
+      </c>
+      <c r="AL107">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="108" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK108">
+        <v>661</v>
+      </c>
+      <c r="AL108">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="109" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK109">
+        <v>661</v>
+      </c>
+      <c r="AL109">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="110" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK110">
+        <v>314</v>
+      </c>
+      <c r="AL110">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="111" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK111">
+        <v>314</v>
+      </c>
+      <c r="AL111">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="112" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK112">
+        <v>390</v>
+      </c>
+      <c r="AL112">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="113" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK113">
+        <v>399</v>
+      </c>
+      <c r="AL113">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="114" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK114">
+        <v>399</v>
+      </c>
+      <c r="AL114">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="115" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK115">
+        <v>399</v>
+      </c>
+      <c r="AL115">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="116" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK116">
+        <v>399</v>
+      </c>
+      <c r="AL116">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="117" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK117">
+        <v>299</v>
+      </c>
+      <c r="AL117">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="118" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK118">
+        <v>131</v>
+      </c>
+      <c r="AL118">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="119" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK119">
+        <v>136</v>
+      </c>
+      <c r="AL119">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="120" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK120">
+        <v>252</v>
+      </c>
+      <c r="AL120">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="121" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK121">
+        <v>313</v>
+      </c>
+      <c r="AL121">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="122" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK122">
+        <v>602</v>
+      </c>
+      <c r="AL122">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="123" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK123">
+        <v>655</v>
+      </c>
+      <c r="AL123">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="124" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK124">
+        <v>242</v>
+      </c>
+      <c r="AL124">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="125" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK125">
+        <v>325</v>
+      </c>
+      <c r="AL125">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="126" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK126">
+        <v>304</v>
+      </c>
+      <c r="AL126">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="127" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK127">
+        <v>513</v>
+      </c>
+      <c r="AL127">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="128" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK128">
+        <v>920</v>
+      </c>
+      <c r="AL128">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="129" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK129">
+        <v>121</v>
+      </c>
+      <c r="AL129">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="130" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK130">
+        <v>269</v>
+      </c>
+      <c r="AL130">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="131" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK131">
+        <v>469</v>
+      </c>
+      <c r="AL131">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="132" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK132">
+        <v>366</v>
+      </c>
+      <c r="AL132">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="133" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK133">
+        <v>363</v>
+      </c>
+      <c r="AL133">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="134" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK134">
+        <v>199</v>
+      </c>
+      <c r="AL134">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="135" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK135">
+        <v>469</v>
+      </c>
+      <c r="AL135">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="136" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK136">
+        <v>326</v>
+      </c>
+      <c r="AL136">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="137" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK137">
+        <v>474</v>
+      </c>
+      <c r="AL137">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="138" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK138">
+        <v>412</v>
+      </c>
+      <c r="AL138">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="139" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK139">
+        <v>445</v>
+      </c>
+      <c r="AL139">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="140" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK140">
+        <v>367</v>
+      </c>
+      <c r="AL140">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="141" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK141">
+        <v>411</v>
+      </c>
+      <c r="AL141">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="142" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK142">
+        <v>508</v>
+      </c>
+      <c r="AL142">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="143" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK143">
+        <v>842</v>
+      </c>
+      <c r="AL143">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="144" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK144">
+        <v>842</v>
+      </c>
+      <c r="AL144">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="145" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK145">
+        <v>842</v>
+      </c>
+      <c r="AL145">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="146" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK146">
+        <v>842</v>
+      </c>
+      <c r="AL146">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="147" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK147">
+        <v>277</v>
+      </c>
+      <c r="AL147">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="148" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK148">
+        <v>292</v>
+      </c>
+      <c r="AL148">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="149" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK149">
+        <v>230</v>
+      </c>
+      <c r="AL149">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="150" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK150">
+        <v>312</v>
+      </c>
+      <c r="AL150">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="151" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK151">
+        <v>357</v>
+      </c>
+      <c r="AL151">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="152" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK152">
+        <v>240</v>
+      </c>
+      <c r="AL152">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="153" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK153">
+        <v>293</v>
+      </c>
+      <c r="AL153">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="154" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK154">
+        <v>293</v>
+      </c>
+      <c r="AL154">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="155" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK155">
+        <v>293</v>
+      </c>
+      <c r="AL155">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="156" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK156">
+        <v>293</v>
+      </c>
+      <c r="AL156">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="157" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK157">
+        <v>293</v>
+      </c>
+      <c r="AL157">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="158" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK158">
+        <v>381</v>
+      </c>
+      <c r="AL158">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="159" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK159">
+        <v>369</v>
+      </c>
+      <c r="AL159">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="160" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK160">
+        <v>369</v>
+      </c>
+      <c r="AL160">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="161" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK161">
+        <v>369</v>
+      </c>
+      <c r="AL161">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="162" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK162">
+        <v>369</v>
+      </c>
+      <c r="AL162">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="163" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK163">
+        <v>369</v>
+      </c>
+      <c r="AL163">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="164" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK164">
+        <v>369</v>
+      </c>
+      <c r="AL164">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="165" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK165">
+        <v>369</v>
+      </c>
+      <c r="AL165">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="166" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK166">
+        <v>369</v>
+      </c>
+      <c r="AL166">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="167" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK167">
+        <v>369</v>
+      </c>
+      <c r="AL167">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="168" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK168">
+        <v>369</v>
+      </c>
+      <c r="AL168">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="169" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK169">
+        <v>369</v>
+      </c>
+      <c r="AL169">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="170" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK170">
+        <v>369</v>
+      </c>
+      <c r="AL170">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="171" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK171">
+        <v>369</v>
+      </c>
+      <c r="AL171">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="172" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK172">
+        <v>369</v>
+      </c>
+      <c r="AL172">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="173" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK173">
+        <v>369</v>
+      </c>
+      <c r="AL173">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="174" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK174">
+        <v>369</v>
+      </c>
+      <c r="AL174">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="175" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK175">
+        <v>369</v>
+      </c>
+      <c r="AL175">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="176" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK176">
+        <v>369</v>
+      </c>
+      <c r="AL176">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="177" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK177">
+        <v>264</v>
+      </c>
+      <c r="AL177">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="178" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK178">
+        <v>264</v>
+      </c>
+      <c r="AL178">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="179" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK179">
+        <v>264</v>
+      </c>
+      <c r="AL179">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="180" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK180">
+        <v>264</v>
+      </c>
+      <c r="AL180">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="181" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK181">
+        <v>264</v>
+      </c>
+      <c r="AL181">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="182" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK182">
+        <v>264</v>
+      </c>
+      <c r="AL182">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="183" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK183">
+        <v>264</v>
+      </c>
+      <c r="AL183">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="184" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK184">
+        <v>264</v>
+      </c>
+      <c r="AL184">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="185" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK185">
+        <v>264</v>
+      </c>
+      <c r="AL185">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="186" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK186">
+        <v>264</v>
+      </c>
+      <c r="AL186">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="187" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK187">
+        <v>264</v>
+      </c>
+      <c r="AL187">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="188" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK188">
+        <v>264</v>
+      </c>
+      <c r="AL188">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="189" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK189">
+        <v>264</v>
+      </c>
+      <c r="AL189">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="190" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK190">
+        <v>264</v>
+      </c>
+      <c r="AL190">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="191" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK191">
+        <v>264</v>
+      </c>
+      <c r="AL191">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="192" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK192">
+        <v>264</v>
+      </c>
+      <c r="AL192">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="193" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK193">
+        <v>264</v>
+      </c>
+      <c r="AL193">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="194" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK194">
+        <v>264</v>
+      </c>
+      <c r="AL194">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="195" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK195">
+        <v>264</v>
+      </c>
+      <c r="AL195">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="196" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK196">
+        <v>264</v>
+      </c>
+      <c r="AL196">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="197" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK197">
+        <v>264</v>
+      </c>
+      <c r="AL197">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="198" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK198">
+        <v>264</v>
+      </c>
+      <c r="AL198">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="199" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK199">
+        <v>264</v>
+      </c>
+      <c r="AL199">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="200" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK200">
+        <v>264</v>
+      </c>
+      <c r="AL200">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="201" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK201">
+        <v>264</v>
+      </c>
+      <c r="AL201">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="202" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK202">
+        <v>339</v>
+      </c>
+      <c r="AL202">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="203" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK203">
+        <v>903</v>
+      </c>
+      <c r="AL203">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="204" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK204">
+        <v>227</v>
+      </c>
+      <c r="AL204">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="205" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK205">
+        <v>600</v>
+      </c>
+      <c r="AL205">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="206" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK206">
+        <v>347</v>
+      </c>
+      <c r="AL206">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="207" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK207">
+        <v>842</v>
+      </c>
+      <c r="AL207">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="208" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK208">
+        <v>353</v>
+      </c>
+      <c r="AL208">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="209" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK209">
+        <v>353</v>
+      </c>
+      <c r="AL209">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="210" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK210">
+        <v>353</v>
+      </c>
+      <c r="AL210">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="211" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK211">
+        <v>353</v>
+      </c>
+      <c r="AL211">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="212" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK212">
+        <v>701</v>
+      </c>
+      <c r="AL212">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="213" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK213">
+        <v>132</v>
+      </c>
+      <c r="AL213">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="214" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK214">
+        <v>191</v>
+      </c>
+      <c r="AL214">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK215">
+        <v>373</v>
+      </c>
+      <c r="AL215">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="216" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK216">
+        <v>150</v>
+      </c>
+      <c r="AL216">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="217" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK217">
+        <v>150</v>
+      </c>
+      <c r="AL217">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="218" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK218">
+        <v>150</v>
+      </c>
+      <c r="AL218">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="219" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK219">
+        <v>150</v>
+      </c>
+      <c r="AL219">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="220" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK220">
+        <v>150</v>
+      </c>
+      <c r="AL220">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="221" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK221">
+        <v>965</v>
+      </c>
+      <c r="AL221">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="222" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK222">
+        <v>369</v>
+      </c>
+      <c r="AL222">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="223" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK223">
+        <v>369</v>
+      </c>
+      <c r="AL223">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="224" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK224">
+        <v>425</v>
+      </c>
+      <c r="AL224">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="225" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK225">
+        <v>508</v>
+      </c>
+      <c r="AL225">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="226" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK226">
+        <v>508</v>
+      </c>
+      <c r="AL226">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="227" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK227">
+        <v>508</v>
+      </c>
+      <c r="AL227">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="228" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK228">
+        <v>508</v>
+      </c>
+      <c r="AL228">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="229" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK229">
+        <v>508</v>
+      </c>
+      <c r="AL229">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="230" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK230">
+        <v>508</v>
+      </c>
+      <c r="AL230">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="231" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK231">
+        <v>508</v>
+      </c>
+      <c r="AL231">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="232" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK232">
+        <v>508</v>
+      </c>
+      <c r="AL232">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="233" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK233">
+        <v>508</v>
+      </c>
+      <c r="AL233">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="234" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK234">
+        <v>508</v>
+      </c>
+      <c r="AL234">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="235" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK235">
+        <v>508</v>
+      </c>
+      <c r="AL235">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="236" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK236">
+        <v>508</v>
+      </c>
+      <c r="AL236">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="237" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK237">
+        <v>508</v>
+      </c>
+      <c r="AL237">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="238" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK238">
+        <v>508</v>
+      </c>
+      <c r="AL238">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="239" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK239">
+        <v>508</v>
+      </c>
+      <c r="AL239">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="240" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK240">
+        <v>508</v>
+      </c>
+      <c r="AL240">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="241" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK241">
+        <v>508</v>
+      </c>
+      <c r="AL241">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="242" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK242">
+        <v>508</v>
+      </c>
+      <c r="AL242">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="243" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK243">
+        <v>508</v>
+      </c>
+      <c r="AL243">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="244" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK244">
+        <v>508</v>
+      </c>
+      <c r="AL244">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="245" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK245">
+        <v>508</v>
+      </c>
+      <c r="AL245">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="246" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK246">
+        <v>508</v>
+      </c>
+      <c r="AL246">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="247" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK247">
+        <v>508</v>
+      </c>
+      <c r="AL247">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="248" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK248">
+        <v>508</v>
+      </c>
+      <c r="AL248">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="249" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK249">
+        <v>508</v>
+      </c>
+      <c r="AL249">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="250" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK250">
+        <v>508</v>
+      </c>
+      <c r="AL250">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="251" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK251">
+        <v>508</v>
+      </c>
+      <c r="AL251">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="252" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK252">
+        <v>508</v>
+      </c>
+      <c r="AL252">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="253" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK253">
+        <v>508</v>
+      </c>
+      <c r="AL253">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="254" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK254">
+        <v>508</v>
+      </c>
+      <c r="AL254">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="255" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK255">
+        <v>508</v>
+      </c>
+      <c r="AL255">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="256" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK256">
+        <v>508</v>
+      </c>
+      <c r="AL256">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="257" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK257">
+        <v>508</v>
+      </c>
+      <c r="AL257">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="258" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK258">
+        <v>508</v>
+      </c>
+      <c r="AL258">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="259" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK259">
+        <v>393</v>
+      </c>
+      <c r="AL259">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="260" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK260">
+        <v>393</v>
+      </c>
+      <c r="AL260">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="261" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK261">
+        <v>393</v>
+      </c>
+      <c r="AL261">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="262" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK262">
+        <v>393</v>
+      </c>
+      <c r="AL262">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="263" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK263">
+        <v>393</v>
+      </c>
+      <c r="AL263">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="264" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK264">
+        <v>393</v>
+      </c>
+      <c r="AL264">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="265" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK265">
+        <v>393</v>
+      </c>
+      <c r="AL265">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="266" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK266">
+        <v>393</v>
+      </c>
+      <c r="AL266">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="267" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK267">
+        <v>393</v>
+      </c>
+      <c r="AL267">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="268" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK268">
+        <v>393</v>
+      </c>
+      <c r="AL268">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="269" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK269">
+        <v>393</v>
+      </c>
+      <c r="AL269">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="270" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK270">
+        <v>393</v>
+      </c>
+      <c r="AL270">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="271" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK271">
+        <v>393</v>
+      </c>
+      <c r="AL271">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="272" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK272">
+        <v>393</v>
+      </c>
+      <c r="AL272">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="273" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK273">
+        <v>393</v>
+      </c>
+      <c r="AL273">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="274" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK274">
+        <v>393</v>
+      </c>
+      <c r="AL274">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="275" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK275">
+        <v>393</v>
+      </c>
+      <c r="AL275">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="276" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK276">
+        <v>393</v>
+      </c>
+      <c r="AL276">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="277" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK277">
+        <v>393</v>
+      </c>
+      <c r="AL277">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="278" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK278">
+        <v>393</v>
+      </c>
+      <c r="AL278">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="279" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK279">
+        <v>393</v>
+      </c>
+      <c r="AL279">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="280" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK280">
+        <v>393</v>
+      </c>
+      <c r="AL280">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="281" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK281">
+        <v>393</v>
+      </c>
+      <c r="AL281">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="282" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK282">
+        <v>339</v>
+      </c>
+      <c r="AL282">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="283" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK283">
+        <v>339</v>
+      </c>
+      <c r="AL283">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="284" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK284">
+        <v>339</v>
+      </c>
+      <c r="AL284">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="285" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK285">
+        <v>339</v>
+      </c>
+      <c r="AL285">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="286" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK286">
+        <v>339</v>
+      </c>
+      <c r="AL286">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="287" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK287">
+        <v>393</v>
+      </c>
+      <c r="AL287">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="288" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK288">
+        <v>373</v>
+      </c>
+      <c r="AL288">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="289" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK289">
+        <v>373</v>
+      </c>
+      <c r="AL289">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="290" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK290">
+        <v>373</v>
+      </c>
+      <c r="AL290">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="291" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK291">
+        <v>373</v>
+      </c>
+      <c r="AL291">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="292" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK292">
+        <v>385</v>
+      </c>
+      <c r="AL292">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="293" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK293">
+        <v>385</v>
+      </c>
+      <c r="AL293">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="294" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK294">
+        <v>385</v>
+      </c>
+      <c r="AL294">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="295" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK295">
+        <v>385</v>
+      </c>
+      <c r="AL295">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="296" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK296">
+        <v>385</v>
+      </c>
+      <c r="AL296">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="297" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK297">
+        <v>385</v>
+      </c>
+      <c r="AL297">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="298" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK298">
+        <v>385</v>
+      </c>
+      <c r="AL298">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="299" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK299">
+        <v>385</v>
+      </c>
+      <c r="AL299">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="300" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK300">
+        <v>385</v>
+      </c>
+      <c r="AL300">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="301" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK301">
+        <v>385</v>
+      </c>
+      <c r="AL301">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="302" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK302">
+        <v>385</v>
+      </c>
+      <c r="AL302">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="303" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK303">
+        <v>385</v>
+      </c>
+      <c r="AL303">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="304" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK304">
+        <v>385</v>
+      </c>
+      <c r="AL304">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="305" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK305">
+        <v>385</v>
+      </c>
+      <c r="AL305">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="306" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK306">
+        <v>385</v>
+      </c>
+      <c r="AL306">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="307" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK307">
+        <v>385</v>
+      </c>
+      <c r="AL307">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="308" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK308">
+        <v>582</v>
+      </c>
+      <c r="AL308">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="309" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK309">
+        <v>582</v>
+      </c>
+      <c r="AL309">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="310" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK310">
+        <v>327</v>
+      </c>
+      <c r="AL310">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="311" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK311">
+        <v>327</v>
+      </c>
+      <c r="AL311">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="312" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK312">
+        <v>327</v>
+      </c>
+      <c r="AL312">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="313" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK313">
+        <v>425</v>
+      </c>
+      <c r="AL313">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="314" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK314">
+        <v>425</v>
+      </c>
+      <c r="AL314">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="315" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK315">
+        <v>425</v>
+      </c>
+      <c r="AL315">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="316" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK316">
+        <v>393</v>
+      </c>
+      <c r="AL316">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="317" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK317">
+        <v>393</v>
+      </c>
+      <c r="AL317">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="318" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK318">
+        <v>701</v>
+      </c>
+      <c r="AL318">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="319" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK319">
+        <v>701</v>
+      </c>
+      <c r="AL319">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="320" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK320">
+        <v>474</v>
+      </c>
+      <c r="AL320">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="321" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK321">
+        <v>474</v>
+      </c>
+      <c r="AL321">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="322" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK322">
+        <v>172</v>
+      </c>
+      <c r="AL322">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="323" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK323">
+        <v>172</v>
+      </c>
+      <c r="AL323">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="324" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK324">
+        <v>172</v>
+      </c>
+      <c r="AL324">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="325" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK325">
+        <v>132</v>
+      </c>
+      <c r="AL325">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="326" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK326">
+        <v>132</v>
+      </c>
+      <c r="AL326">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="327" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK327">
+        <v>351</v>
+      </c>
+      <c r="AL327">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="328" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK328">
+        <v>351</v>
+      </c>
+      <c r="AL328">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="329" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK329">
+        <v>351</v>
+      </c>
+      <c r="AL329">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="330" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK330">
+        <v>1409</v>
+      </c>
+      <c r="AL330">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="331" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK331">
+        <v>1409</v>
+      </c>
+      <c r="AL331">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="332" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK332">
+        <v>580</v>
+      </c>
+      <c r="AL332">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="333" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK333">
+        <v>276</v>
+      </c>
+      <c r="AL333">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="334" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK334">
+        <v>309</v>
+      </c>
+      <c r="AL334">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="335" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK335">
+        <v>316</v>
+      </c>
+      <c r="AL335">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="336" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK336">
+        <v>278</v>
+      </c>
+      <c r="AL336">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="337" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK337">
+        <v>380</v>
+      </c>
+      <c r="AL337">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="338" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK338">
+        <v>847</v>
+      </c>
+      <c r="AL338">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="339" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK339">
+        <v>842</v>
+      </c>
+      <c r="AL339">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="340" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK340">
+        <v>334</v>
+      </c>
+      <c r="AL340">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="341" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK341">
+        <v>385</v>
+      </c>
+      <c r="AL341">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="342" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK342">
+        <v>532</v>
+      </c>
+      <c r="AL342">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="343" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK343">
+        <v>191</v>
+      </c>
+      <c r="AL343">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="344" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK344">
+        <v>842</v>
+      </c>
+      <c r="AL344">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="345" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK345">
+        <v>308</v>
+      </c>
+      <c r="AL345">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="346" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK346">
+        <v>309</v>
+      </c>
+      <c r="AL346">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="347" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK347">
+        <v>688</v>
+      </c>
+      <c r="AL347">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="348" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK348">
+        <v>419</v>
+      </c>
+      <c r="AL348">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="349" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK349">
+        <v>504</v>
+      </c>
+      <c r="AL349">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="350" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK350">
+        <v>170</v>
+      </c>
+      <c r="AL350">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="351" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK351">
+        <v>533</v>
+      </c>
+      <c r="AL351">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="352" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK352">
+        <v>266</v>
+      </c>
+      <c r="AL352">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="353" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK353">
+        <v>334</v>
+      </c>
+      <c r="AL353">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="354" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK354">
+        <v>327</v>
+      </c>
+      <c r="AL354">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="355" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK355">
+        <v>360</v>
+      </c>
+      <c r="AL355">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="356" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK356">
+        <v>323</v>
+      </c>
+      <c r="AL356">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="357" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK357">
+        <v>375</v>
+      </c>
+      <c r="AL357">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="358" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK358">
+        <v>429</v>
+      </c>
+      <c r="AL358">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="359" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK359">
+        <v>410</v>
+      </c>
+      <c r="AL359">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="360" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK360">
+        <v>603</v>
+      </c>
+      <c r="AL360">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="361" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK361">
+        <v>603</v>
+      </c>
+      <c r="AL361">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="362" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK362">
+        <v>369</v>
+      </c>
+      <c r="AL362">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="363" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK363">
+        <v>309</v>
+      </c>
+      <c r="AL363">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="364" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK364">
+        <v>360</v>
+      </c>
+      <c r="AL364">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="365" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK365">
+        <v>592</v>
+      </c>
+      <c r="AL365">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="366" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK366">
+        <v>1409</v>
+      </c>
+      <c r="AL366">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="367" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK367">
+        <v>436</v>
+      </c>
+      <c r="AL367">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="368" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK368">
+        <v>265</v>
+      </c>
+      <c r="AL368">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="369" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK369">
+        <v>360</v>
+      </c>
+      <c r="AL369">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="370" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK370">
+        <v>410</v>
+      </c>
+      <c r="AL370">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="371" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK371">
+        <v>242</v>
+      </c>
+      <c r="AL371">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="372" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK372">
+        <v>242</v>
+      </c>
+      <c r="AL372">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="373" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK373">
+        <v>366</v>
+      </c>
+      <c r="AL373">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="374" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK374">
+        <v>366</v>
+      </c>
+      <c r="AL374">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="375" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK375">
+        <v>327</v>
+      </c>
+      <c r="AL375">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="376" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK376">
+        <v>614</v>
+      </c>
+      <c r="AL376">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="377" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK377">
+        <v>310</v>
+      </c>
+      <c r="AL377">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="378" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK378">
+        <v>320</v>
+      </c>
+      <c r="AL378">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="379" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK379">
+        <v>379</v>
+      </c>
+      <c r="AL379">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="380" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK380">
+        <v>501</v>
+      </c>
+      <c r="AL380">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="381" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK381">
+        <v>690</v>
+      </c>
+      <c r="AL381">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="382" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK382">
+        <v>163</v>
+      </c>
+      <c r="AL382">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="383" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK383">
+        <v>233</v>
+      </c>
+      <c r="AL383">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="384" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK384">
+        <v>233</v>
+      </c>
+      <c r="AL384">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="385" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK385">
+        <v>375</v>
+      </c>
+      <c r="AL385">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="386" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK386">
+        <v>375</v>
+      </c>
+      <c r="AL386">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="387" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK387">
+        <v>375</v>
+      </c>
+      <c r="AL387">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="388" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK388">
+        <v>375</v>
+      </c>
+      <c r="AL388">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="389" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK389">
+        <v>375</v>
+      </c>
+      <c r="AL389">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="390" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK390">
+        <v>375</v>
+      </c>
+      <c r="AL390">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="391" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK391">
+        <v>375</v>
+      </c>
+      <c r="AL391">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="392" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK392">
+        <v>375</v>
+      </c>
+      <c r="AL392">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="393" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK393">
+        <v>375</v>
+      </c>
+      <c r="AL393">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="394" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK394">
+        <v>375</v>
+      </c>
+      <c r="AL394">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="395" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK395">
+        <v>269</v>
+      </c>
+      <c r="AL395">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="396" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK396">
+        <v>269</v>
+      </c>
+      <c r="AL396">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="397" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK397">
+        <v>456</v>
+      </c>
+      <c r="AL397">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="398" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK398">
+        <v>456</v>
+      </c>
+      <c r="AL398">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="399" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK399">
+        <v>429</v>
+      </c>
+      <c r="AL399">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="400" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK400">
+        <v>429</v>
+      </c>
+      <c r="AL400">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="401" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK401">
+        <v>429</v>
+      </c>
+      <c r="AL401">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="402" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK402">
+        <v>429</v>
+      </c>
+      <c r="AL402">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="403" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK403">
+        <v>495</v>
+      </c>
+      <c r="AL403">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="404" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK404">
+        <v>303</v>
+      </c>
+      <c r="AL404">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="405" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK405">
+        <v>233</v>
+      </c>
+      <c r="AL405">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="406" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK406">
+        <v>233</v>
+      </c>
+      <c r="AL406">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="407" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK407">
+        <v>233</v>
+      </c>
+      <c r="AL407">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="408" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK408">
+        <v>233</v>
+      </c>
+      <c r="AL408">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="409" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK409">
+        <v>233</v>
+      </c>
+      <c r="AL409">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="410" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK410">
+        <v>115</v>
+      </c>
+      <c r="AL410">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="411" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK411">
+        <v>373</v>
+      </c>
+      <c r="AL411">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="412" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK412">
+        <v>373</v>
+      </c>
+      <c r="AL412">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="413" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK413">
+        <v>383</v>
+      </c>
+      <c r="AL413">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="414" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK414">
+        <v>383</v>
+      </c>
+      <c r="AL414">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="415" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK415">
+        <v>296</v>
+      </c>
+      <c r="AL415">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="416" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK416">
+        <v>571</v>
+      </c>
+      <c r="AL416">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="417" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK417">
+        <v>571</v>
+      </c>
+      <c r="AL417">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="418" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK418">
+        <v>495</v>
+      </c>
+      <c r="AL418">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="419" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK419">
+        <v>495</v>
+      </c>
+      <c r="AL419">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="420" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK420">
+        <v>363</v>
+      </c>
+      <c r="AL420">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="421" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK421">
+        <v>363</v>
+      </c>
+      <c r="AL421">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="422" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK422">
+        <v>520</v>
+      </c>
+      <c r="AL422">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="423" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK423">
+        <v>429</v>
+      </c>
+      <c r="AL423">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="424" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK424">
+        <v>633</v>
+      </c>
+      <c r="AL424">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="425" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK425">
+        <v>199</v>
+      </c>
+      <c r="AL425">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="426" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK426">
+        <v>347</v>
+      </c>
+      <c r="AL426">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="427" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK427">
+        <v>304</v>
+      </c>
+      <c r="AL427">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="428" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK428">
+        <v>927</v>
+      </c>
+      <c r="AL428">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="429" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK429">
+        <v>278</v>
+      </c>
+      <c r="AL429">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="430" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK430">
+        <v>411</v>
+      </c>
+      <c r="AL430">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="431" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK431">
+        <v>411</v>
+      </c>
+      <c r="AL431">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="432" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK432">
+        <v>411</v>
+      </c>
+      <c r="AL432">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="433" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK433">
+        <v>347</v>
+      </c>
+      <c r="AL433">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="434" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK434">
+        <v>347</v>
+      </c>
+      <c r="AL434">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="435" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK435">
+        <v>365</v>
+      </c>
+      <c r="AL435">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="436" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK436">
+        <v>650</v>
+      </c>
+      <c r="AL436">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="437" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK437">
+        <v>385</v>
+      </c>
+      <c r="AL437">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="438" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK438">
+        <v>512</v>
+      </c>
+      <c r="AL438">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="439" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK439">
+        <v>506</v>
+      </c>
+      <c r="AL439">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="440" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK440">
+        <v>508</v>
+      </c>
+      <c r="AL440">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="441" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK441">
+        <v>323</v>
+      </c>
+      <c r="AL441">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="442" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK442">
+        <v>842</v>
+      </c>
+      <c r="AL442">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="443" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK443">
+        <v>326</v>
+      </c>
+      <c r="AL443">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="444" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK444">
+        <v>882</v>
+      </c>
+      <c r="AL444">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="445" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK445">
+        <v>882</v>
+      </c>
+      <c r="AL445">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="446" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK446">
+        <v>842</v>
+      </c>
+      <c r="AL446">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="447" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK447">
+        <v>842</v>
+      </c>
+      <c r="AL447">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="448" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK448">
+        <v>842</v>
+      </c>
+      <c r="AL448">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="449" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK449">
+        <v>842</v>
+      </c>
+      <c r="AL449">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="450" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK450">
+        <v>842</v>
+      </c>
+      <c r="AL450">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="451" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK451">
+        <v>842</v>
+      </c>
+      <c r="AL451">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="452" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK452">
+        <v>842</v>
+      </c>
+      <c r="AL452">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="453" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK453">
+        <v>842</v>
+      </c>
+      <c r="AL453">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="454" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK454">
+        <v>842</v>
+      </c>
+      <c r="AL454">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="455" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK455">
+        <v>842</v>
+      </c>
+      <c r="AL455">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="456" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK456">
+        <v>379</v>
+      </c>
+      <c r="AL456">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="457" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK457">
+        <v>842</v>
+      </c>
+      <c r="AL457">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="458" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK458">
+        <v>842</v>
+      </c>
+      <c r="AL458">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="459" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK459">
+        <v>842</v>
+      </c>
+      <c r="AL459">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="460" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK460">
+        <v>842</v>
+      </c>
+      <c r="AL460">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="461" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK461">
+        <v>842</v>
+      </c>
+      <c r="AL461">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="462" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK462">
+        <v>842</v>
+      </c>
+      <c r="AL462">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="463" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK463">
+        <v>842</v>
+      </c>
+      <c r="AL463">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="464" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK464">
+        <v>842</v>
+      </c>
+      <c r="AL464">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="465" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK465">
+        <v>842</v>
+      </c>
+      <c r="AL465">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="466" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK466">
+        <v>842</v>
+      </c>
+      <c r="AL466">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="467" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK467">
+        <v>339</v>
+      </c>
+      <c r="AL467">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="468" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK468">
+        <v>338</v>
+      </c>
+      <c r="AL468">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="469" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK469">
+        <v>790</v>
+      </c>
+      <c r="AL469">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="470" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK470">
+        <v>790</v>
+      </c>
+      <c r="AL470">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="471" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK471">
+        <v>582</v>
+      </c>
+      <c r="AL471">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="472" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK472">
+        <v>582</v>
+      </c>
+      <c r="AL472">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="473" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK473">
+        <v>309</v>
+      </c>
+      <c r="AL473">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="474" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK474">
+        <v>309</v>
+      </c>
+      <c r="AL474">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="475" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK475">
+        <v>577</v>
+      </c>
+      <c r="AL475">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="476" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK476">
+        <v>292</v>
+      </c>
+      <c r="AL476">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="477" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK477">
+        <v>334</v>
+      </c>
+      <c r="AL477">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="478" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK478">
+        <v>334</v>
+      </c>
+      <c r="AL478">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="479" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK479">
+        <v>329</v>
+      </c>
+      <c r="AL479">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="480" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK480">
+        <v>385</v>
+      </c>
+      <c r="AL480">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="481" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK481">
+        <v>339</v>
+      </c>
+      <c r="AL481">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="482" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK482">
+        <v>179</v>
+      </c>
+      <c r="AL482">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="483" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK483">
+        <v>508</v>
+      </c>
+      <c r="AL483">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="484" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK484">
+        <v>508</v>
+      </c>
+      <c r="AL484">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="485" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK485">
+        <v>508</v>
+      </c>
+      <c r="AL485">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="486" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK486">
+        <v>394</v>
+      </c>
+      <c r="AL486">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="487" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK487">
+        <v>324</v>
+      </c>
+      <c r="AL487">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="488" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK488">
+        <v>266</v>
+      </c>
+      <c r="AL488">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="489" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK489">
+        <v>339</v>
+      </c>
+      <c r="AL489">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="490" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK490">
+        <v>367</v>
+      </c>
+      <c r="AL490">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="491" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK491">
+        <v>441</v>
+      </c>
+      <c r="AL491">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="492" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK492">
+        <v>504</v>
+      </c>
+      <c r="AL492">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="493" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK493">
+        <v>265</v>
+      </c>
+      <c r="AL493">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="494" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK494">
+        <v>393</v>
+      </c>
+      <c r="AL494">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="495" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK495">
+        <v>393</v>
+      </c>
+      <c r="AL495">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="496" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK496">
+        <v>181</v>
+      </c>
+      <c r="AL496">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="497" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK497">
+        <v>181</v>
+      </c>
+      <c r="AL497">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="498" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK498">
+        <v>181</v>
+      </c>
+      <c r="AL498">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="499" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK499">
+        <v>181</v>
+      </c>
+      <c r="AL499">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="500" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK500">
+        <v>181</v>
+      </c>
+      <c r="AL500">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="501" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK501">
+        <v>859</v>
+      </c>
+      <c r="AL501">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="502" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK502">
+        <v>1124</v>
+      </c>
+      <c r="AL502">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="503" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK503">
+        <v>859</v>
+      </c>
+      <c r="AL503">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="504" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK504">
+        <v>859</v>
+      </c>
+      <c r="AL504">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="505" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK505">
+        <v>1160</v>
+      </c>
+      <c r="AL505">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="506" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK506">
+        <v>859</v>
+      </c>
+      <c r="AL506">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="507" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK507">
+        <v>429</v>
+      </c>
+      <c r="AL507">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="508" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK508">
+        <v>429</v>
+      </c>
+      <c r="AL508">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="509" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK509">
+        <v>429</v>
+      </c>
+      <c r="AL509">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="510" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK510">
+        <v>429</v>
+      </c>
+      <c r="AL510">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="511" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK511">
+        <v>429</v>
+      </c>
+      <c r="AL511">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="512" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK512">
+        <v>429</v>
+      </c>
+      <c r="AL512">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="513" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK513">
+        <v>429</v>
+      </c>
+      <c r="AL513">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="514" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK514">
+        <v>429</v>
+      </c>
+      <c r="AL514">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="515" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK515">
+        <v>429</v>
+      </c>
+      <c r="AL515">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="516" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK516">
+        <v>429</v>
+      </c>
+      <c r="AL516">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="517" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK517">
+        <v>429</v>
+      </c>
+      <c r="AL517">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="518" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK518">
+        <v>429</v>
+      </c>
+      <c r="AL518">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="519" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK519">
+        <v>429</v>
+      </c>
+      <c r="AL519">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="520" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK520">
+        <v>429</v>
+      </c>
+      <c r="AL520">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="521" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK521">
+        <v>429</v>
+      </c>
+      <c r="AL521">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="522" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK522">
+        <v>429</v>
+      </c>
+      <c r="AL522">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="523" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK523">
+        <v>429</v>
+      </c>
+      <c r="AL523">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="524" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK524">
+        <v>429</v>
+      </c>
+      <c r="AL524">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="525" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK525">
+        <v>429</v>
+      </c>
+      <c r="AL525">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="526" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK526">
+        <v>429</v>
+      </c>
+      <c r="AL526">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="527" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK527">
+        <v>429</v>
+      </c>
+      <c r="AL527">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="528" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK528">
+        <v>429</v>
+      </c>
+      <c r="AL528">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="529" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK529">
+        <v>566</v>
+      </c>
+      <c r="AL529">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="530" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK530">
+        <v>566</v>
+      </c>
+      <c r="AL530">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="531" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK531">
+        <v>566</v>
+      </c>
+      <c r="AL531">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="532" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK532">
+        <v>863</v>
+      </c>
+      <c r="AL532">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="533" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK533">
+        <v>677</v>
+      </c>
+      <c r="AL533">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="534" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK534">
+        <v>325</v>
+      </c>
+      <c r="AL534">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="535" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK535">
+        <v>571</v>
+      </c>
+      <c r="AL535">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="536" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK536">
+        <v>154</v>
+      </c>
+      <c r="AL536">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="537" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK537">
+        <v>339</v>
+      </c>
+      <c r="AL537">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="538" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK538">
+        <v>282</v>
+      </c>
+      <c r="AL538">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="539" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK539">
+        <v>495</v>
+      </c>
+      <c r="AL539">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="540" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK540">
+        <v>439</v>
+      </c>
+      <c r="AL540">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="541" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK541">
+        <v>321</v>
+      </c>
+      <c r="AL541">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="542" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK542">
+        <v>321</v>
+      </c>
+      <c r="AL542">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="543" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK543">
+        <v>321</v>
+      </c>
+      <c r="AL543">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="544" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK544">
+        <v>321</v>
+      </c>
+      <c r="AL544">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="545" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK545">
+        <v>321</v>
+      </c>
+      <c r="AL545">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="546" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK546">
+        <v>321</v>
+      </c>
+      <c r="AL546">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="547" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK547">
+        <v>321</v>
+      </c>
+      <c r="AL547">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="548" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK548">
+        <v>684</v>
+      </c>
+      <c r="AL548">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="549" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK549">
+        <v>242</v>
+      </c>
+      <c r="AL549">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="550" spans="37:38" x14ac:dyDescent="0.25">
+      <c r="AK550">
+        <v>368</v>
+      </c>
+      <c r="AL550">
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>